<commit_message>
PEP8 changes and active directory test
Further PEP8 changes and a new test to replace manual testing of active
directory import/remove
</commit_message>
<xml_diff>
--- a/aimautomation/src/root/nested/resources/import_configuration.xlsx
+++ b/aimautomation/src/root/nested/resources/import_configuration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="10860" windowHeight="6960" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11685" windowHeight="7020" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AIM setup" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <definedName name="TXNAME">Transmitters!$F$6:$F$6</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <oleSize ref="A1:G18"/>
+  <oleSize ref="A1:H17"/>
 </workbook>
 </file>
 
@@ -1000,6 +1000,20 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1013,20 +1027,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1984,7 +1984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C6" sqref="C6:M6"/>
     </sheetView>
@@ -2275,9 +2275,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HW10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2881,429 +2881,429 @@
       </c>
     </row>
     <row r="2" spans="2:102" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="64" t="s">
         <v>101</v>
       </c>
       <c r="C2" s="17"/>
     </row>
     <row r="3" spans="2:102" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="60"/>
+      <c r="B3" s="64"/>
     </row>
     <row r="4" spans="2:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="60"/>
+      <c r="B4" s="64"/>
     </row>
     <row r="5" spans="2:102" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="61"/>
-      <c r="C5" s="62" t="s">
+      <c r="B5" s="65"/>
+      <c r="C5" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="62" t="s">
+      <c r="D5" s="61"/>
+      <c r="E5" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="63"/>
-      <c r="G5" s="62" t="s">
+      <c r="F5" s="61"/>
+      <c r="G5" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="63"/>
-      <c r="I5" s="62" t="s">
+      <c r="H5" s="61"/>
+      <c r="I5" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="63"/>
-      <c r="K5" s="62" t="s">
+      <c r="J5" s="61"/>
+      <c r="K5" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="63"/>
-      <c r="M5" s="62" t="s">
+      <c r="L5" s="61"/>
+      <c r="M5" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="63"/>
-      <c r="O5" s="62" t="s">
+      <c r="N5" s="61"/>
+      <c r="O5" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="63"/>
-      <c r="Q5" s="62" t="s">
+      <c r="P5" s="61"/>
+      <c r="Q5" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="R5" s="63"/>
-      <c r="S5" s="62" t="s">
+      <c r="R5" s="61"/>
+      <c r="S5" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="T5" s="63"/>
-      <c r="U5" s="62" t="s">
+      <c r="T5" s="61"/>
+      <c r="U5" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="V5" s="63"/>
-      <c r="W5" s="62" t="s">
+      <c r="V5" s="61"/>
+      <c r="W5" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="X5" s="63"/>
-      <c r="Y5" s="62" t="s">
+      <c r="X5" s="61"/>
+      <c r="Y5" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="Z5" s="63"/>
-      <c r="AA5" s="62" t="s">
+      <c r="Z5" s="61"/>
+      <c r="AA5" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="AB5" s="63"/>
-      <c r="AC5" s="62" t="s">
+      <c r="AB5" s="61"/>
+      <c r="AC5" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="AD5" s="63"/>
-      <c r="AE5" s="62" t="s">
+      <c r="AD5" s="61"/>
+      <c r="AE5" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="AF5" s="63"/>
-      <c r="AG5" s="62" t="s">
+      <c r="AF5" s="61"/>
+      <c r="AG5" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="AH5" s="63"/>
-      <c r="AI5" s="62" t="s">
+      <c r="AH5" s="61"/>
+      <c r="AI5" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="AJ5" s="63"/>
-      <c r="AK5" s="62" t="s">
+      <c r="AJ5" s="61"/>
+      <c r="AK5" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="AL5" s="63"/>
-      <c r="AM5" s="62" t="s">
+      <c r="AL5" s="61"/>
+      <c r="AM5" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="AN5" s="63"/>
-      <c r="AO5" s="62" t="s">
+      <c r="AN5" s="61"/>
+      <c r="AO5" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="AP5" s="63"/>
-      <c r="AQ5" s="62" t="s">
+      <c r="AP5" s="61"/>
+      <c r="AQ5" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="AR5" s="63"/>
-      <c r="AS5" s="62" t="s">
+      <c r="AR5" s="61"/>
+      <c r="AS5" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="AT5" s="63"/>
-      <c r="AU5" s="62" t="s">
+      <c r="AT5" s="61"/>
+      <c r="AU5" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="AV5" s="63"/>
-      <c r="AW5" s="62" t="s">
+      <c r="AV5" s="61"/>
+      <c r="AW5" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="AX5" s="63"/>
-      <c r="AY5" s="62" t="s">
+      <c r="AX5" s="61"/>
+      <c r="AY5" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="AZ5" s="63"/>
-      <c r="BA5" s="62" t="s">
+      <c r="AZ5" s="61"/>
+      <c r="BA5" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="BB5" s="63"/>
-      <c r="BC5" s="62" t="s">
+      <c r="BB5" s="61"/>
+      <c r="BC5" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="BD5" s="63"/>
-      <c r="BE5" s="62" t="s">
+      <c r="BD5" s="61"/>
+      <c r="BE5" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="BF5" s="63"/>
-      <c r="BG5" s="62" t="s">
+      <c r="BF5" s="61"/>
+      <c r="BG5" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="BH5" s="63"/>
-      <c r="BI5" s="62" t="s">
+      <c r="BH5" s="61"/>
+      <c r="BI5" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="BJ5" s="63"/>
-      <c r="BK5" s="62" t="s">
+      <c r="BJ5" s="61"/>
+      <c r="BK5" s="60" t="s">
         <v>76</v>
       </c>
-      <c r="BL5" s="63"/>
-      <c r="BM5" s="62" t="s">
+      <c r="BL5" s="61"/>
+      <c r="BM5" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="BN5" s="63"/>
-      <c r="BO5" s="62" t="s">
+      <c r="BN5" s="61"/>
+      <c r="BO5" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="BP5" s="63"/>
-      <c r="BQ5" s="62" t="s">
+      <c r="BP5" s="61"/>
+      <c r="BQ5" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="BR5" s="63"/>
-      <c r="BS5" s="62" t="s">
+      <c r="BR5" s="61"/>
+      <c r="BS5" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="BT5" s="63"/>
-      <c r="BU5" s="62" t="s">
+      <c r="BT5" s="61"/>
+      <c r="BU5" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="BV5" s="63"/>
-      <c r="BW5" s="62" t="s">
+      <c r="BV5" s="61"/>
+      <c r="BW5" s="60" t="s">
         <v>82</v>
       </c>
-      <c r="BX5" s="63"/>
-      <c r="BY5" s="62" t="s">
+      <c r="BX5" s="61"/>
+      <c r="BY5" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="BZ5" s="63"/>
-      <c r="CA5" s="62" t="s">
+      <c r="BZ5" s="61"/>
+      <c r="CA5" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="CB5" s="63"/>
-      <c r="CC5" s="62" t="s">
+      <c r="CB5" s="61"/>
+      <c r="CC5" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="CD5" s="63"/>
-      <c r="CE5" s="62" t="s">
+      <c r="CD5" s="61"/>
+      <c r="CE5" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="CF5" s="63"/>
-      <c r="CG5" s="62" t="s">
+      <c r="CF5" s="61"/>
+      <c r="CG5" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="CH5" s="63"/>
-      <c r="CI5" s="62" t="s">
+      <c r="CH5" s="61"/>
+      <c r="CI5" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="CJ5" s="63"/>
-      <c r="CK5" s="62" t="s">
+      <c r="CJ5" s="61"/>
+      <c r="CK5" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="CL5" s="63"/>
-      <c r="CM5" s="62" t="s">
+      <c r="CL5" s="61"/>
+      <c r="CM5" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="CN5" s="63"/>
-      <c r="CO5" s="62" t="s">
+      <c r="CN5" s="61"/>
+      <c r="CO5" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="CP5" s="63"/>
-      <c r="CQ5" s="62" t="s">
+      <c r="CP5" s="61"/>
+      <c r="CQ5" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="CR5" s="63"/>
-      <c r="CS5" s="62" t="s">
+      <c r="CR5" s="61"/>
+      <c r="CS5" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="CT5" s="63"/>
-      <c r="CU5" s="62" t="s">
+      <c r="CT5" s="61"/>
+      <c r="CU5" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="CV5" s="63"/>
-      <c r="CW5" s="62" t="s">
+      <c r="CV5" s="61"/>
+      <c r="CW5" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="CX5" s="63"/>
+      <c r="CX5" s="61"/>
     </row>
     <row r="6" spans="2:102" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="59"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="59"/>
-      <c r="U6" s="58"/>
-      <c r="V6" s="59"/>
-      <c r="W6" s="58"/>
-      <c r="X6" s="59"/>
-      <c r="Y6" s="58"/>
-      <c r="Z6" s="59"/>
-      <c r="AA6" s="58"/>
-      <c r="AB6" s="59"/>
-      <c r="AC6" s="58"/>
-      <c r="AD6" s="59"/>
-      <c r="AE6" s="58"/>
-      <c r="AF6" s="59"/>
-      <c r="AG6" s="58"/>
-      <c r="AH6" s="59"/>
-      <c r="AI6" s="58"/>
-      <c r="AJ6" s="59"/>
-      <c r="AK6" s="58"/>
-      <c r="AL6" s="59"/>
-      <c r="AM6" s="58"/>
-      <c r="AN6" s="59"/>
-      <c r="AO6" s="58"/>
-      <c r="AP6" s="59"/>
-      <c r="AQ6" s="58"/>
-      <c r="AR6" s="59"/>
-      <c r="AS6" s="58"/>
-      <c r="AT6" s="59"/>
-      <c r="AU6" s="58"/>
-      <c r="AV6" s="59"/>
-      <c r="AW6" s="58"/>
-      <c r="AX6" s="59"/>
-      <c r="AY6" s="58"/>
-      <c r="AZ6" s="59"/>
-      <c r="BA6" s="58"/>
-      <c r="BB6" s="59"/>
-      <c r="BC6" s="58"/>
-      <c r="BD6" s="59"/>
-      <c r="BE6" s="58"/>
-      <c r="BF6" s="59"/>
-      <c r="BG6" s="58"/>
-      <c r="BH6" s="59"/>
-      <c r="BI6" s="58"/>
-      <c r="BJ6" s="59"/>
-      <c r="BK6" s="58"/>
-      <c r="BL6" s="59"/>
-      <c r="BM6" s="58"/>
-      <c r="BN6" s="59"/>
-      <c r="BO6" s="58"/>
-      <c r="BP6" s="59"/>
-      <c r="BQ6" s="58"/>
-      <c r="BR6" s="59"/>
-      <c r="BS6" s="58"/>
-      <c r="BT6" s="59"/>
-      <c r="BU6" s="58"/>
-      <c r="BV6" s="59"/>
-      <c r="BW6" s="58"/>
-      <c r="BX6" s="59"/>
-      <c r="BY6" s="58"/>
-      <c r="BZ6" s="59"/>
-      <c r="CA6" s="58"/>
-      <c r="CB6" s="59"/>
-      <c r="CC6" s="58"/>
-      <c r="CD6" s="59"/>
-      <c r="CE6" s="58"/>
-      <c r="CF6" s="59"/>
-      <c r="CG6" s="58"/>
-      <c r="CH6" s="59"/>
-      <c r="CI6" s="58"/>
-      <c r="CJ6" s="59"/>
-      <c r="CK6" s="58"/>
-      <c r="CL6" s="59"/>
-      <c r="CM6" s="58"/>
-      <c r="CN6" s="59"/>
-      <c r="CO6" s="58"/>
-      <c r="CP6" s="59"/>
-      <c r="CQ6" s="58"/>
-      <c r="CR6" s="59"/>
-      <c r="CS6" s="58"/>
-      <c r="CT6" s="59"/>
-      <c r="CU6" s="58"/>
-      <c r="CV6" s="59"/>
-      <c r="CW6" s="58"/>
-      <c r="CX6" s="59"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="62"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="62"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="62"/>
+      <c r="V6" s="63"/>
+      <c r="W6" s="62"/>
+      <c r="X6" s="63"/>
+      <c r="Y6" s="62"/>
+      <c r="Z6" s="63"/>
+      <c r="AA6" s="62"/>
+      <c r="AB6" s="63"/>
+      <c r="AC6" s="62"/>
+      <c r="AD6" s="63"/>
+      <c r="AE6" s="62"/>
+      <c r="AF6" s="63"/>
+      <c r="AG6" s="62"/>
+      <c r="AH6" s="63"/>
+      <c r="AI6" s="62"/>
+      <c r="AJ6" s="63"/>
+      <c r="AK6" s="62"/>
+      <c r="AL6" s="63"/>
+      <c r="AM6" s="62"/>
+      <c r="AN6" s="63"/>
+      <c r="AO6" s="62"/>
+      <c r="AP6" s="63"/>
+      <c r="AQ6" s="62"/>
+      <c r="AR6" s="63"/>
+      <c r="AS6" s="62"/>
+      <c r="AT6" s="63"/>
+      <c r="AU6" s="62"/>
+      <c r="AV6" s="63"/>
+      <c r="AW6" s="62"/>
+      <c r="AX6" s="63"/>
+      <c r="AY6" s="62"/>
+      <c r="AZ6" s="63"/>
+      <c r="BA6" s="62"/>
+      <c r="BB6" s="63"/>
+      <c r="BC6" s="62"/>
+      <c r="BD6" s="63"/>
+      <c r="BE6" s="62"/>
+      <c r="BF6" s="63"/>
+      <c r="BG6" s="62"/>
+      <c r="BH6" s="63"/>
+      <c r="BI6" s="62"/>
+      <c r="BJ6" s="63"/>
+      <c r="BK6" s="62"/>
+      <c r="BL6" s="63"/>
+      <c r="BM6" s="62"/>
+      <c r="BN6" s="63"/>
+      <c r="BO6" s="62"/>
+      <c r="BP6" s="63"/>
+      <c r="BQ6" s="62"/>
+      <c r="BR6" s="63"/>
+      <c r="BS6" s="62"/>
+      <c r="BT6" s="63"/>
+      <c r="BU6" s="62"/>
+      <c r="BV6" s="63"/>
+      <c r="BW6" s="62"/>
+      <c r="BX6" s="63"/>
+      <c r="BY6" s="62"/>
+      <c r="BZ6" s="63"/>
+      <c r="CA6" s="62"/>
+      <c r="CB6" s="63"/>
+      <c r="CC6" s="62"/>
+      <c r="CD6" s="63"/>
+      <c r="CE6" s="62"/>
+      <c r="CF6" s="63"/>
+      <c r="CG6" s="62"/>
+      <c r="CH6" s="63"/>
+      <c r="CI6" s="62"/>
+      <c r="CJ6" s="63"/>
+      <c r="CK6" s="62"/>
+      <c r="CL6" s="63"/>
+      <c r="CM6" s="62"/>
+      <c r="CN6" s="63"/>
+      <c r="CO6" s="62"/>
+      <c r="CP6" s="63"/>
+      <c r="CQ6" s="62"/>
+      <c r="CR6" s="63"/>
+      <c r="CS6" s="62"/>
+      <c r="CT6" s="63"/>
+      <c r="CU6" s="62"/>
+      <c r="CV6" s="63"/>
+      <c r="CW6" s="62"/>
+      <c r="CX6" s="63"/>
     </row>
     <row r="7" spans="2:102" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="65"/>
-      <c r="O7" s="64"/>
-      <c r="P7" s="65"/>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="65"/>
-      <c r="S7" s="64"/>
-      <c r="T7" s="65"/>
-      <c r="U7" s="64"/>
-      <c r="V7" s="65"/>
-      <c r="W7" s="64"/>
-      <c r="X7" s="65"/>
-      <c r="Y7" s="64"/>
-      <c r="Z7" s="65"/>
-      <c r="AA7" s="64"/>
-      <c r="AB7" s="65"/>
-      <c r="AC7" s="64"/>
-      <c r="AD7" s="65"/>
-      <c r="AE7" s="64"/>
-      <c r="AF7" s="65"/>
-      <c r="AG7" s="64"/>
-      <c r="AH7" s="65"/>
-      <c r="AI7" s="64"/>
-      <c r="AJ7" s="65"/>
-      <c r="AK7" s="64"/>
-      <c r="AL7" s="65"/>
-      <c r="AM7" s="64"/>
-      <c r="AN7" s="65"/>
-      <c r="AO7" s="64"/>
-      <c r="AP7" s="65"/>
-      <c r="AQ7" s="64"/>
-      <c r="AR7" s="65"/>
-      <c r="AS7" s="64"/>
-      <c r="AT7" s="65"/>
-      <c r="AU7" s="64"/>
-      <c r="AV7" s="65"/>
-      <c r="AW7" s="64"/>
-      <c r="AX7" s="65"/>
-      <c r="AY7" s="64"/>
-      <c r="AZ7" s="65"/>
-      <c r="BA7" s="64"/>
-      <c r="BB7" s="65"/>
-      <c r="BC7" s="64"/>
-      <c r="BD7" s="65"/>
-      <c r="BE7" s="64"/>
-      <c r="BF7" s="65"/>
-      <c r="BG7" s="64"/>
-      <c r="BH7" s="65"/>
-      <c r="BI7" s="64"/>
-      <c r="BJ7" s="65"/>
-      <c r="BK7" s="64"/>
-      <c r="BL7" s="65"/>
-      <c r="BM7" s="64"/>
-      <c r="BN7" s="65"/>
-      <c r="BO7" s="64"/>
-      <c r="BP7" s="65"/>
-      <c r="BQ7" s="64"/>
-      <c r="BR7" s="65"/>
-      <c r="BS7" s="64"/>
-      <c r="BT7" s="65"/>
-      <c r="BU7" s="64"/>
-      <c r="BV7" s="65"/>
-      <c r="BW7" s="64"/>
-      <c r="BX7" s="65"/>
-      <c r="BY7" s="64"/>
-      <c r="BZ7" s="65"/>
-      <c r="CA7" s="64"/>
-      <c r="CB7" s="65"/>
-      <c r="CC7" s="64"/>
-      <c r="CD7" s="65"/>
-      <c r="CE7" s="64"/>
-      <c r="CF7" s="65"/>
-      <c r="CG7" s="64"/>
-      <c r="CH7" s="65"/>
-      <c r="CI7" s="64"/>
-      <c r="CJ7" s="65"/>
-      <c r="CK7" s="64"/>
-      <c r="CL7" s="65"/>
-      <c r="CM7" s="64"/>
-      <c r="CN7" s="65"/>
-      <c r="CO7" s="64"/>
-      <c r="CP7" s="65"/>
-      <c r="CQ7" s="64"/>
-      <c r="CR7" s="65"/>
-      <c r="CS7" s="64"/>
-      <c r="CT7" s="65"/>
-      <c r="CU7" s="64"/>
-      <c r="CV7" s="65"/>
-      <c r="CW7" s="64"/>
-      <c r="CX7" s="65"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="58"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="59"/>
+      <c r="S7" s="58"/>
+      <c r="T7" s="59"/>
+      <c r="U7" s="58"/>
+      <c r="V7" s="59"/>
+      <c r="W7" s="58"/>
+      <c r="X7" s="59"/>
+      <c r="Y7" s="58"/>
+      <c r="Z7" s="59"/>
+      <c r="AA7" s="58"/>
+      <c r="AB7" s="59"/>
+      <c r="AC7" s="58"/>
+      <c r="AD7" s="59"/>
+      <c r="AE7" s="58"/>
+      <c r="AF7" s="59"/>
+      <c r="AG7" s="58"/>
+      <c r="AH7" s="59"/>
+      <c r="AI7" s="58"/>
+      <c r="AJ7" s="59"/>
+      <c r="AK7" s="58"/>
+      <c r="AL7" s="59"/>
+      <c r="AM7" s="58"/>
+      <c r="AN7" s="59"/>
+      <c r="AO7" s="58"/>
+      <c r="AP7" s="59"/>
+      <c r="AQ7" s="58"/>
+      <c r="AR7" s="59"/>
+      <c r="AS7" s="58"/>
+      <c r="AT7" s="59"/>
+      <c r="AU7" s="58"/>
+      <c r="AV7" s="59"/>
+      <c r="AW7" s="58"/>
+      <c r="AX7" s="59"/>
+      <c r="AY7" s="58"/>
+      <c r="AZ7" s="59"/>
+      <c r="BA7" s="58"/>
+      <c r="BB7" s="59"/>
+      <c r="BC7" s="58"/>
+      <c r="BD7" s="59"/>
+      <c r="BE7" s="58"/>
+      <c r="BF7" s="59"/>
+      <c r="BG7" s="58"/>
+      <c r="BH7" s="59"/>
+      <c r="BI7" s="58"/>
+      <c r="BJ7" s="59"/>
+      <c r="BK7" s="58"/>
+      <c r="BL7" s="59"/>
+      <c r="BM7" s="58"/>
+      <c r="BN7" s="59"/>
+      <c r="BO7" s="58"/>
+      <c r="BP7" s="59"/>
+      <c r="BQ7" s="58"/>
+      <c r="BR7" s="59"/>
+      <c r="BS7" s="58"/>
+      <c r="BT7" s="59"/>
+      <c r="BU7" s="58"/>
+      <c r="BV7" s="59"/>
+      <c r="BW7" s="58"/>
+      <c r="BX7" s="59"/>
+      <c r="BY7" s="58"/>
+      <c r="BZ7" s="59"/>
+      <c r="CA7" s="58"/>
+      <c r="CB7" s="59"/>
+      <c r="CC7" s="58"/>
+      <c r="CD7" s="59"/>
+      <c r="CE7" s="58"/>
+      <c r="CF7" s="59"/>
+      <c r="CG7" s="58"/>
+      <c r="CH7" s="59"/>
+      <c r="CI7" s="58"/>
+      <c r="CJ7" s="59"/>
+      <c r="CK7" s="58"/>
+      <c r="CL7" s="59"/>
+      <c r="CM7" s="58"/>
+      <c r="CN7" s="59"/>
+      <c r="CO7" s="58"/>
+      <c r="CP7" s="59"/>
+      <c r="CQ7" s="58"/>
+      <c r="CR7" s="59"/>
+      <c r="CS7" s="58"/>
+      <c r="CT7" s="59"/>
+      <c r="CU7" s="58"/>
+      <c r="CV7" s="59"/>
+      <c r="CW7" s="58"/>
+      <c r="CX7" s="59"/>
     </row>
     <row r="8" spans="2:102" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C8" s="19" t="s">
@@ -13810,90 +13810,49 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="151">
-    <mergeCell ref="CO7:CP7"/>
-    <mergeCell ref="CQ7:CR7"/>
-    <mergeCell ref="CS7:CT7"/>
-    <mergeCell ref="CU7:CV7"/>
-    <mergeCell ref="CW7:CX7"/>
-    <mergeCell ref="CE7:CF7"/>
-    <mergeCell ref="CG7:CH7"/>
-    <mergeCell ref="CI7:CJ7"/>
-    <mergeCell ref="CK7:CL7"/>
-    <mergeCell ref="CM7:CN7"/>
-    <mergeCell ref="BU7:BV7"/>
-    <mergeCell ref="BW7:BX7"/>
-    <mergeCell ref="BY7:BZ7"/>
-    <mergeCell ref="CA7:CB7"/>
-    <mergeCell ref="CC7:CD7"/>
-    <mergeCell ref="BK7:BL7"/>
-    <mergeCell ref="BM7:BN7"/>
-    <mergeCell ref="BO7:BP7"/>
-    <mergeCell ref="BQ7:BR7"/>
-    <mergeCell ref="BS7:BT7"/>
-    <mergeCell ref="BA7:BB7"/>
-    <mergeCell ref="BC7:BD7"/>
-    <mergeCell ref="BE7:BF7"/>
-    <mergeCell ref="BG7:BH7"/>
-    <mergeCell ref="BI7:BJ7"/>
-    <mergeCell ref="AQ7:AR7"/>
-    <mergeCell ref="AS7:AT7"/>
-    <mergeCell ref="AU7:AV7"/>
-    <mergeCell ref="AW7:AX7"/>
-    <mergeCell ref="AY7:AZ7"/>
-    <mergeCell ref="AG7:AH7"/>
-    <mergeCell ref="AI7:AJ7"/>
-    <mergeCell ref="AK7:AL7"/>
-    <mergeCell ref="AM7:AN7"/>
-    <mergeCell ref="AO7:AP7"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AW5:AX5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AG5:AH5"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="CW5:CX5"/>
-    <mergeCell ref="CK5:CL5"/>
-    <mergeCell ref="CM5:CN5"/>
-    <mergeCell ref="CO5:CP5"/>
-    <mergeCell ref="CQ5:CR5"/>
-    <mergeCell ref="CU5:CV5"/>
-    <mergeCell ref="CA5:CB5"/>
-    <mergeCell ref="CC5:CD5"/>
-    <mergeCell ref="CE5:CF5"/>
-    <mergeCell ref="CG5:CH5"/>
-    <mergeCell ref="CI5:CJ5"/>
-    <mergeCell ref="CS5:CT5"/>
+    <mergeCell ref="CU6:CV6"/>
+    <mergeCell ref="CW6:CX6"/>
+    <mergeCell ref="CI6:CJ6"/>
+    <mergeCell ref="CK6:CL6"/>
+    <mergeCell ref="CM6:CN6"/>
+    <mergeCell ref="CO6:CP6"/>
+    <mergeCell ref="CQ6:CR6"/>
+    <mergeCell ref="CS6:CT6"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="BA6:BB6"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="BE6:BF6"/>
+    <mergeCell ref="BG6:BH6"/>
+    <mergeCell ref="CG6:CH6"/>
+    <mergeCell ref="BK6:BL6"/>
+    <mergeCell ref="BM6:BN6"/>
+    <mergeCell ref="BO6:BP6"/>
+    <mergeCell ref="BQ6:BR6"/>
+    <mergeCell ref="BS6:BT6"/>
+    <mergeCell ref="BU6:BV6"/>
+    <mergeCell ref="BW6:BX6"/>
+    <mergeCell ref="BY6:BZ6"/>
+    <mergeCell ref="CA6:CB6"/>
+    <mergeCell ref="CC6:CD6"/>
+    <mergeCell ref="CE6:CF6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AG6:AH6"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="M6:N6"/>
     <mergeCell ref="BY5:BZ5"/>
     <mergeCell ref="BK5:BL5"/>
     <mergeCell ref="BI6:BJ6"/>
@@ -13918,49 +13877,90 @@
     <mergeCell ref="BG5:BH5"/>
     <mergeCell ref="BO5:BP5"/>
     <mergeCell ref="BQ5:BR5"/>
-    <mergeCell ref="CE6:CF6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AG6:AH6"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="CU6:CV6"/>
-    <mergeCell ref="CW6:CX6"/>
-    <mergeCell ref="CI6:CJ6"/>
-    <mergeCell ref="CK6:CL6"/>
-    <mergeCell ref="CM6:CN6"/>
-    <mergeCell ref="CO6:CP6"/>
-    <mergeCell ref="CQ6:CR6"/>
-    <mergeCell ref="CS6:CT6"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="BA6:BB6"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="BE6:BF6"/>
-    <mergeCell ref="BG6:BH6"/>
-    <mergeCell ref="CG6:CH6"/>
-    <mergeCell ref="BK6:BL6"/>
-    <mergeCell ref="BM6:BN6"/>
-    <mergeCell ref="BO6:BP6"/>
-    <mergeCell ref="BQ6:BR6"/>
-    <mergeCell ref="BS6:BT6"/>
-    <mergeCell ref="BU6:BV6"/>
-    <mergeCell ref="BW6:BX6"/>
-    <mergeCell ref="BY6:BZ6"/>
-    <mergeCell ref="CA6:CB6"/>
-    <mergeCell ref="CC6:CD6"/>
+    <mergeCell ref="CW5:CX5"/>
+    <mergeCell ref="CK5:CL5"/>
+    <mergeCell ref="CM5:CN5"/>
+    <mergeCell ref="CO5:CP5"/>
+    <mergeCell ref="CQ5:CR5"/>
+    <mergeCell ref="CU5:CV5"/>
+    <mergeCell ref="CA5:CB5"/>
+    <mergeCell ref="CC5:CD5"/>
+    <mergeCell ref="CE5:CF5"/>
+    <mergeCell ref="CG5:CH5"/>
+    <mergeCell ref="CI5:CJ5"/>
+    <mergeCell ref="CS5:CT5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AW5:AX5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="AG7:AH7"/>
+    <mergeCell ref="AI7:AJ7"/>
+    <mergeCell ref="AK7:AL7"/>
+    <mergeCell ref="AM7:AN7"/>
+    <mergeCell ref="AO7:AP7"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="BA7:BB7"/>
+    <mergeCell ref="BC7:BD7"/>
+    <mergeCell ref="BE7:BF7"/>
+    <mergeCell ref="BG7:BH7"/>
+    <mergeCell ref="BI7:BJ7"/>
+    <mergeCell ref="AQ7:AR7"/>
+    <mergeCell ref="AS7:AT7"/>
+    <mergeCell ref="AU7:AV7"/>
+    <mergeCell ref="AW7:AX7"/>
+    <mergeCell ref="AY7:AZ7"/>
+    <mergeCell ref="BU7:BV7"/>
+    <mergeCell ref="BW7:BX7"/>
+    <mergeCell ref="BY7:BZ7"/>
+    <mergeCell ref="CA7:CB7"/>
+    <mergeCell ref="CC7:CD7"/>
+    <mergeCell ref="BK7:BL7"/>
+    <mergeCell ref="BM7:BN7"/>
+    <mergeCell ref="BO7:BP7"/>
+    <mergeCell ref="BQ7:BR7"/>
+    <mergeCell ref="BS7:BT7"/>
+    <mergeCell ref="CO7:CP7"/>
+    <mergeCell ref="CQ7:CR7"/>
+    <mergeCell ref="CS7:CT7"/>
+    <mergeCell ref="CU7:CV7"/>
+    <mergeCell ref="CW7:CX7"/>
+    <mergeCell ref="CE7:CF7"/>
+    <mergeCell ref="CG7:CH7"/>
+    <mergeCell ref="CI7:CJ7"/>
+    <mergeCell ref="CK7:CL7"/>
+    <mergeCell ref="CM7:CN7"/>
   </mergeCells>
   <conditionalFormatting sqref="B1 B2:C2">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>